<commit_message>
Update README and project files
</commit_message>
<xml_diff>
--- a/Bus_Dicts_Exams.xlsx
+++ b/Bus_Dicts_Exams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João\Ambiente de Trabalho\DW_National_Exams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaovieira/Desktop/DW_National_Exams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF71C58F-66A1-455B-9229-0C0E515D99A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05797A8F-C491-2641-AC7C-7E4169EBD135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="142">
   <si>
     <t>Data Mart</t>
   </si>
@@ -218,15 +218,6 @@
   </si>
   <si>
     <t>CourseType</t>
-  </si>
-  <si>
-    <t>analytic Grade</t>
-  </si>
-  <si>
-    <t>analytic Intern Final Classification</t>
-  </si>
-  <si>
-    <t>analytic Final Classification of the Course</t>
   </si>
   <si>
     <t>analytic Grade of Exam By Examenee Demographic and Phase</t>
@@ -786,10 +777,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,22 +1085,21 @@
   </sheetPr>
   <dimension ref="C3:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="6.77734375" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" customWidth="1"/>
     <col min="9" max="9" width="6" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" customWidth="1"/>
-    <col min="11" max="11" width="5.21875" customWidth="1"/>
-    <col min="12" max="15" width="5.77734375" customWidth="1"/>
+    <col min="10" max="11" width="5.1640625" customWidth="1"/>
+    <col min="12" max="15" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" ht="115.8" customHeight="1">
+    <row r="3" spans="3:14" ht="115.75" customHeight="1">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1137,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="3:14" ht="13.2">
+    <row r="4" spans="3:14" ht="13">
       <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1177,7 +1167,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="3:14" ht="13.2">
+    <row r="5" spans="3:14" ht="13">
       <c r="C5" s="5"/>
       <c r="D5" s="35" t="s">
         <v>15</v>
@@ -1193,7 +1183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="3:14" ht="13.2">
+    <row r="6" spans="3:14" ht="13">
       <c r="C6" s="5"/>
       <c r="D6" s="31" t="s">
         <v>16</v>
@@ -1216,7 +1206,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="3:14" ht="13.2">
+    <row r="7" spans="3:14" ht="13">
       <c r="C7" s="5"/>
       <c r="D7" s="31" t="s">
         <v>17</v>
@@ -1240,7 +1230,7 @@
       </c>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="3:14" ht="13.2">
+    <row r="8" spans="3:14" ht="13">
       <c r="C8" s="5"/>
       <c r="D8" s="31" t="s">
         <v>18</v>
@@ -1265,7 +1255,7 @@
       </c>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="3:14" ht="13.2">
+    <row r="9" spans="3:14" ht="13">
       <c r="D9" s="31" t="s">
         <v>19</v>
       </c>
@@ -1288,36 +1278,36 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="3:14" ht="13.2">
+    <row r="10" spans="3:14" ht="13">
       <c r="C10" s="5"/>
     </row>
-    <row r="13" spans="3:14" ht="13.2">
+    <row r="13" spans="3:14" ht="13">
       <c r="C13" s="14"/>
     </row>
-    <row r="14" spans="3:14" ht="13.2">
+    <row r="14" spans="3:14" ht="13">
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="3:14" ht="13.2">
+    <row r="15" spans="3:14" ht="13">
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="3:14" ht="13.2">
+    <row r="16" spans="3:14" ht="13">
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="3:6" ht="13.2">
+    <row r="17" spans="3:6" ht="13">
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="3:6" ht="13.2">
+    <row r="18" spans="3:6" ht="13">
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="3:6" ht="13.2">
+    <row r="19" spans="3:6" ht="13">
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="3:6" ht="13.2">
+    <row r="20" spans="3:6" ht="13">
       <c r="F20" s="14"/>
     </row>
   </sheetData>
@@ -1342,16 +1332,18 @@
   </sheetPr>
   <dimension ref="B2:X49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24">
+    <row r="2" spans="2:24" ht="15.75" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1410,7 +1402,7 @@
         <v>45737</v>
       </c>
     </row>
-    <row r="3" spans="2:24">
+    <row r="3" spans="2:24" ht="15.75" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1445,7 +1437,7 @@
       <c r="W3" s="36"/>
       <c r="X3" s="32"/>
     </row>
-    <row r="4" spans="2:24">
+    <row r="4" spans="2:24" ht="15.75" customHeight="1">
       <c r="B4" s="37" t="s">
         <v>27</v>
       </c>
@@ -1455,7 +1447,7 @@
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
       <c r="H4" s="32"/>
-      <c r="J4" s="40" t="s">
+      <c r="J4" s="41" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="36"/>
@@ -1474,7 +1466,7 @@
       <c r="W4" s="36"/>
       <c r="X4" s="32"/>
     </row>
-    <row r="5" spans="2:24">
+    <row r="5" spans="2:24" ht="15.75" customHeight="1">
       <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
@@ -1509,7 +1501,7 @@
       <c r="W5" s="36"/>
       <c r="X5" s="32"/>
     </row>
-    <row r="6" spans="2:24">
+    <row r="6" spans="2:24" ht="15.75" customHeight="1">
       <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
@@ -1544,7 +1536,7 @@
       <c r="W6" s="36"/>
       <c r="X6" s="32"/>
     </row>
-    <row r="7" spans="2:24">
+    <row r="7" spans="2:24" ht="15.75" customHeight="1">
       <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
@@ -1579,7 +1571,7 @@
       <c r="W7" s="36"/>
       <c r="X7" s="32"/>
     </row>
-    <row r="8" spans="2:24">
+    <row r="8" spans="2:24" ht="15.75" customHeight="1">
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -1591,7 +1583,7 @@
       <c r="F8" s="36"/>
       <c r="G8" s="36"/>
       <c r="H8" s="32"/>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="41" t="s">
         <v>28</v>
       </c>
       <c r="K8" s="36"/>
@@ -1612,7 +1604,7 @@
       <c r="W8" s="36"/>
       <c r="X8" s="32"/>
     </row>
-    <row r="9" spans="2:24">
+    <row r="9" spans="2:24" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
         <v>10</v>
       </c>
@@ -1645,7 +1637,7 @@
       <c r="W9" s="36"/>
       <c r="X9" s="32"/>
     </row>
-    <row r="10" spans="2:24">
+    <row r="10" spans="2:24" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
@@ -1680,7 +1672,7 @@
       <c r="W10" s="36"/>
       <c r="X10" s="32"/>
     </row>
-    <row r="11" spans="2:24">
+    <row r="11" spans="2:24" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
         <v>33</v>
       </c>
@@ -1715,7 +1707,7 @@
       <c r="W11" s="36"/>
       <c r="X11" s="32"/>
     </row>
-    <row r="12" spans="2:24">
+    <row r="12" spans="2:24" ht="15.75" customHeight="1">
       <c r="B12" s="15" t="s">
         <v>37</v>
       </c>
@@ -1750,7 +1742,7 @@
       <c r="W12" s="36"/>
       <c r="X12" s="32"/>
     </row>
-    <row r="13" spans="2:24">
+    <row r="13" spans="2:24" ht="15.75" customHeight="1">
       <c r="B13" s="15" t="s">
         <v>40</v>
       </c>
@@ -1785,7 +1777,7 @@
       <c r="W13" s="36"/>
       <c r="X13" s="32"/>
     </row>
-    <row r="14" spans="2:24">
+    <row r="14" spans="2:24" ht="15.75" customHeight="1">
       <c r="B14" s="15" t="s">
         <v>43</v>
       </c>
@@ -1820,7 +1812,7 @@
       <c r="W14" s="36"/>
       <c r="X14" s="32"/>
     </row>
-    <row r="15" spans="2:24">
+    <row r="15" spans="2:24" ht="15.75" customHeight="1">
       <c r="B15" s="15" t="s">
         <v>46</v>
       </c>
@@ -1855,7 +1847,7 @@
       <c r="W15" s="36"/>
       <c r="X15" s="32"/>
     </row>
-    <row r="16" spans="2:24">
+    <row r="16" spans="2:24" ht="15.75" customHeight="1">
       <c r="B16" s="37" t="s">
         <v>28</v>
       </c>
@@ -1877,7 +1869,7 @@
       <c r="W16" s="36"/>
       <c r="X16" s="32"/>
     </row>
-    <row r="17" spans="2:24">
+    <row r="17" spans="2:24" ht="15.75" customHeight="1">
       <c r="B17" s="15" t="s">
         <v>29</v>
       </c>
@@ -1890,7 +1882,7 @@
       <c r="G17" s="36"/>
       <c r="H17" s="32"/>
     </row>
-    <row r="18" spans="2:24">
+    <row r="18" spans="2:24" ht="15.75" customHeight="1">
       <c r="B18" s="15" t="s">
         <v>31</v>
       </c>
@@ -1903,7 +1895,7 @@
       <c r="G18" s="36"/>
       <c r="H18" s="32"/>
     </row>
-    <row r="19" spans="2:24">
+    <row r="19" spans="2:24" ht="15.75" customHeight="1">
       <c r="B19" s="15" t="s">
         <v>35</v>
       </c>
@@ -1954,7 +1946,7 @@
         <v>45738</v>
       </c>
     </row>
-    <row r="20" spans="2:24">
+    <row r="20" spans="2:24" ht="15.75" customHeight="1">
       <c r="J20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1978,7 +1970,7 @@
       <c r="W20" s="36"/>
       <c r="X20" s="32"/>
     </row>
-    <row r="21" spans="2:24">
+    <row r="21" spans="2:24" ht="15.75" customHeight="1">
       <c r="J21" s="37" t="s">
         <v>27</v>
       </c>
@@ -1998,7 +1990,7 @@
       <c r="W21" s="36"/>
       <c r="X21" s="32"/>
     </row>
-    <row r="22" spans="2:24">
+    <row r="22" spans="2:24" ht="15.75" customHeight="1">
       <c r="J22" s="15" t="s">
         <v>3</v>
       </c>
@@ -2022,7 +2014,7 @@
       <c r="W22" s="36"/>
       <c r="X22" s="32"/>
     </row>
-    <row r="23" spans="2:24">
+    <row r="23" spans="2:24" ht="15.75" customHeight="1">
       <c r="J23" s="15" t="s">
         <v>5</v>
       </c>
@@ -2046,7 +2038,7 @@
       <c r="W23" s="36"/>
       <c r="X23" s="32"/>
     </row>
-    <row r="24" spans="2:24">
+    <row r="24" spans="2:24" ht="15.75" customHeight="1">
       <c r="J24" s="15" t="s">
         <v>9</v>
       </c>
@@ -2070,11 +2062,11 @@
       <c r="W24" s="36"/>
       <c r="X24" s="32"/>
     </row>
-    <row r="25" spans="2:24">
+    <row r="25" spans="2:24" ht="15.75" customHeight="1">
       <c r="J25" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="K25" s="41" t="s">
+      <c r="K25" s="38" t="s">
         <v>55</v>
       </c>
       <c r="L25" s="36"/>
@@ -2094,7 +2086,7 @@
       <c r="W25" s="36"/>
       <c r="X25" s="32"/>
     </row>
-    <row r="26" spans="2:24">
+    <row r="26" spans="2:24" ht="15.75" customHeight="1">
       <c r="J26" s="37" t="s">
         <v>28</v>
       </c>
@@ -2116,17 +2108,17 @@
       <c r="W26" s="36"/>
       <c r="X26" s="32"/>
     </row>
-    <row r="27" spans="2:24">
+    <row r="27" spans="2:24" ht="15.75" customHeight="1">
       <c r="J27" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K27" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="39"/>
+      <c r="K27" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="40"/>
+      <c r="O27" s="40"/>
       <c r="P27" s="34"/>
       <c r="R27" s="37" t="s">
         <v>28</v>
@@ -2138,12 +2130,12 @@
       <c r="W27" s="36"/>
       <c r="X27" s="32"/>
     </row>
-    <row r="28" spans="2:24">
+    <row r="28" spans="2:24" ht="15.75" customHeight="1">
       <c r="J28" s="15" t="s">
         <v>31</v>
       </c>
       <c r="K28" s="31" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="36"/>
@@ -2153,21 +2145,21 @@
       <c r="R28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="S28" s="38" t="s">
+      <c r="S28" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="T28" s="39"/>
-      <c r="U28" s="39"/>
-      <c r="V28" s="39"/>
-      <c r="W28" s="39"/>
+      <c r="T28" s="40"/>
+      <c r="U28" s="40"/>
+      <c r="V28" s="40"/>
+      <c r="W28" s="40"/>
       <c r="X28" s="34"/>
     </row>
-    <row r="29" spans="2:24">
+    <row r="29" spans="2:24" ht="15.75" customHeight="1">
       <c r="J29" s="15" t="s">
         <v>35</v>
       </c>
       <c r="K29" s="31" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="L29" s="36"/>
       <c r="M29" s="36"/>
@@ -2186,7 +2178,7 @@
       <c r="W29" s="36"/>
       <c r="X29" s="32"/>
     </row>
-    <row r="30" spans="2:24">
+    <row r="30" spans="2:24" ht="15.75" customHeight="1">
       <c r="J30" s="15" t="s">
         <v>38</v>
       </c>
@@ -2210,7 +2202,7 @@
       <c r="W30" s="36"/>
       <c r="X30" s="32"/>
     </row>
-    <row r="31" spans="2:24">
+    <row r="31" spans="2:24" ht="15.75" customHeight="1">
       <c r="J31" s="15" t="s">
         <v>41</v>
       </c>
@@ -2234,7 +2226,7 @@
       <c r="W31" s="36"/>
       <c r="X31" s="32"/>
     </row>
-    <row r="32" spans="2:24">
+    <row r="32" spans="2:24" ht="15.75" customHeight="1">
       <c r="J32" s="15" t="s">
         <v>44</v>
       </c>
@@ -2258,7 +2250,7 @@
       <c r="W32" s="36"/>
       <c r="X32" s="32"/>
     </row>
-    <row r="33" spans="10:24">
+    <row r="33" spans="10:24" ht="15.75" customHeight="1">
       <c r="J33" s="15" t="s">
         <v>47</v>
       </c>
@@ -2282,7 +2274,7 @@
       <c r="W33" s="36"/>
       <c r="X33" s="32"/>
     </row>
-    <row r="34" spans="10:24">
+    <row r="34" spans="10:24" ht="13">
       <c r="R34" s="15" t="s">
         <v>47</v>
       </c>
@@ -2295,7 +2287,7 @@
       <c r="W34" s="36"/>
       <c r="X34" s="32"/>
     </row>
-    <row r="35" spans="10:24">
+    <row r="35" spans="10:24" ht="13">
       <c r="J35" s="1" t="s">
         <v>20</v>
       </c>
@@ -2316,12 +2308,12 @@
         <v>45738</v>
       </c>
     </row>
-    <row r="36" spans="10:24">
+    <row r="36" spans="10:24" ht="13">
       <c r="J36" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K36" s="31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L36" s="36"/>
       <c r="M36" s="36"/>
@@ -2329,7 +2321,7 @@
       <c r="O36" s="36"/>
       <c r="P36" s="32"/>
     </row>
-    <row r="37" spans="10:24">
+    <row r="37" spans="10:24" ht="13">
       <c r="J37" s="37" t="s">
         <v>27</v>
       </c>
@@ -2340,7 +2332,7 @@
       <c r="O37" s="36"/>
       <c r="P37" s="32"/>
     </row>
-    <row r="38" spans="10:24">
+    <row r="38" spans="10:24" ht="13">
       <c r="J38" s="15" t="s">
         <v>3</v>
       </c>
@@ -2353,7 +2345,7 @@
       <c r="O38" s="36"/>
       <c r="P38" s="32"/>
     </row>
-    <row r="39" spans="10:24">
+    <row r="39" spans="10:24" ht="13">
       <c r="J39" s="15" t="s">
         <v>55</v>
       </c>
@@ -2366,7 +2358,7 @@
       <c r="O39" s="36"/>
       <c r="P39" s="32"/>
     </row>
-    <row r="40" spans="10:24">
+    <row r="40" spans="10:24" ht="13">
       <c r="J40" s="15" t="s">
         <v>11</v>
       </c>
@@ -2379,7 +2371,7 @@
       <c r="O40" s="36"/>
       <c r="P40" s="32"/>
     </row>
-    <row r="41" spans="10:24">
+    <row r="41" spans="10:24" ht="13">
       <c r="J41" s="15" t="s">
         <v>9</v>
       </c>
@@ -2392,7 +2384,7 @@
       <c r="O41" s="36"/>
       <c r="P41" s="32"/>
     </row>
-    <row r="42" spans="10:24">
+    <row r="42" spans="10:24" ht="13">
       <c r="J42" s="37" t="s">
         <v>28</v>
       </c>
@@ -2403,20 +2395,20 @@
       <c r="O42" s="36"/>
       <c r="P42" s="32"/>
     </row>
-    <row r="43" spans="10:24">
+    <row r="43" spans="10:24" ht="13">
       <c r="J43" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K43" s="38" t="s">
+      <c r="K43" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="39"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="40"/>
+      <c r="N43" s="40"/>
+      <c r="O43" s="40"/>
       <c r="P43" s="34"/>
     </row>
-    <row r="44" spans="10:24">
+    <row r="44" spans="10:24" ht="13">
       <c r="J44" s="15" t="s">
         <v>31</v>
       </c>
@@ -2429,7 +2421,7 @@
       <c r="O44" s="36"/>
       <c r="P44" s="32"/>
     </row>
-    <row r="45" spans="10:24">
+    <row r="45" spans="10:24" ht="13">
       <c r="J45" s="15" t="s">
         <v>35</v>
       </c>
@@ -2442,7 +2434,7 @@
       <c r="O45" s="36"/>
       <c r="P45" s="32"/>
     </row>
-    <row r="46" spans="10:24">
+    <row r="46" spans="10:24" ht="13">
       <c r="J46" s="15" t="s">
         <v>38</v>
       </c>
@@ -2455,7 +2447,7 @@
       <c r="O46" s="36"/>
       <c r="P46" s="32"/>
     </row>
-    <row r="47" spans="10:24">
+    <row r="47" spans="10:24" ht="13">
       <c r="J47" s="15" t="s">
         <v>41</v>
       </c>
@@ -2468,7 +2460,7 @@
       <c r="O47" s="36"/>
       <c r="P47" s="32"/>
     </row>
-    <row r="48" spans="10:24">
+    <row r="48" spans="10:24" ht="13">
       <c r="J48" s="15" t="s">
         <v>44</v>
       </c>
@@ -2481,7 +2473,7 @@
       <c r="O48" s="36"/>
       <c r="P48" s="32"/>
     </row>
-    <row r="49" spans="10:16">
+    <row r="49" spans="10:16" ht="13">
       <c r="J49" s="15" t="s">
         <v>47</v>
       </c>
@@ -2496,63 +2488,27 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="K15:P15"/>
-    <mergeCell ref="K20:P20"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="K22:P22"/>
-    <mergeCell ref="K23:P23"/>
-    <mergeCell ref="K24:P24"/>
-    <mergeCell ref="K25:P25"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="K27:P27"/>
-    <mergeCell ref="K28:P28"/>
-    <mergeCell ref="K29:P29"/>
-    <mergeCell ref="K30:P30"/>
-    <mergeCell ref="K31:P31"/>
-    <mergeCell ref="K32:P32"/>
-    <mergeCell ref="K33:P33"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:P36"/>
-    <mergeCell ref="J37:P37"/>
-    <mergeCell ref="K45:P45"/>
-    <mergeCell ref="K46:P46"/>
-    <mergeCell ref="K47:P47"/>
-    <mergeCell ref="K48:P48"/>
-    <mergeCell ref="K49:P49"/>
-    <mergeCell ref="K38:P38"/>
-    <mergeCell ref="K39:P39"/>
-    <mergeCell ref="K40:P40"/>
-    <mergeCell ref="K41:P41"/>
-    <mergeCell ref="J42:P42"/>
-    <mergeCell ref="K43:P43"/>
-    <mergeCell ref="K44:P44"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="K3:P3"/>
-    <mergeCell ref="S3:X3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="S5:X5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="S31:X31"/>
+    <mergeCell ref="S32:X32"/>
+    <mergeCell ref="S33:X33"/>
+    <mergeCell ref="S34:X34"/>
+    <mergeCell ref="S22:X22"/>
+    <mergeCell ref="S23:X23"/>
+    <mergeCell ref="S24:X24"/>
+    <mergeCell ref="S25:X25"/>
+    <mergeCell ref="S26:X26"/>
+    <mergeCell ref="R27:X27"/>
+    <mergeCell ref="S28:X28"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:X20"/>
+    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="S29:X29"/>
+    <mergeCell ref="S30:X30"/>
+    <mergeCell ref="S12:X12"/>
+    <mergeCell ref="S13:X13"/>
+    <mergeCell ref="S14:X14"/>
+    <mergeCell ref="S15:X15"/>
+    <mergeCell ref="S16:X16"/>
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="K10:P10"/>
     <mergeCell ref="K11:P11"/>
@@ -2568,27 +2524,63 @@
     <mergeCell ref="J8:P8"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="K9:P9"/>
-    <mergeCell ref="S12:X12"/>
-    <mergeCell ref="S13:X13"/>
-    <mergeCell ref="S14:X14"/>
-    <mergeCell ref="S15:X15"/>
-    <mergeCell ref="S16:X16"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:X20"/>
-    <mergeCell ref="R21:X21"/>
-    <mergeCell ref="S29:X29"/>
-    <mergeCell ref="S30:X30"/>
-    <mergeCell ref="S31:X31"/>
-    <mergeCell ref="S32:X32"/>
-    <mergeCell ref="S33:X33"/>
-    <mergeCell ref="S34:X34"/>
-    <mergeCell ref="S22:X22"/>
-    <mergeCell ref="S23:X23"/>
-    <mergeCell ref="S24:X24"/>
-    <mergeCell ref="S25:X25"/>
-    <mergeCell ref="S26:X26"/>
-    <mergeCell ref="R27:X27"/>
-    <mergeCell ref="S28:X28"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="S5:X5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="K3:P3"/>
+    <mergeCell ref="S3:X3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="K48:P48"/>
+    <mergeCell ref="K49:P49"/>
+    <mergeCell ref="K38:P38"/>
+    <mergeCell ref="K39:P39"/>
+    <mergeCell ref="K40:P40"/>
+    <mergeCell ref="K41:P41"/>
+    <mergeCell ref="J42:P42"/>
+    <mergeCell ref="K43:P43"/>
+    <mergeCell ref="K44:P44"/>
+    <mergeCell ref="K36:P36"/>
+    <mergeCell ref="J37:P37"/>
+    <mergeCell ref="K45:P45"/>
+    <mergeCell ref="K46:P46"/>
+    <mergeCell ref="K47:P47"/>
+    <mergeCell ref="K30:P30"/>
+    <mergeCell ref="K31:P31"/>
+    <mergeCell ref="K32:P32"/>
+    <mergeCell ref="K33:P33"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K25:P25"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="K27:P27"/>
+    <mergeCell ref="K28:P28"/>
+    <mergeCell ref="K29:P29"/>
+    <mergeCell ref="K20:P20"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="K22:P22"/>
+    <mergeCell ref="K23:P23"/>
+    <mergeCell ref="K24:P24"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="K15:P15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2603,26 +2595,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="9.21875" customWidth="1"/>
-    <col min="14" max="14" width="11.88671875" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" customWidth="1"/>
+    <col min="15" max="15" width="7.83203125" customWidth="1"/>
     <col min="16" max="16" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16">
+    <row r="2" spans="2:16" ht="15.75" customHeight="1">
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2631,21 +2623,21 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" ht="15.75" customHeight="1">
       <c r="B3" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>22</v>
@@ -2654,19 +2646,19 @@
         <v>45738</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M3" s="17" t="s">
         <v>21</v>
       </c>
       <c r="N3" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O3" s="17" t="s">
         <v>22</v>
@@ -2675,18 +2667,18 @@
         <v>45738</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" ht="15.75" customHeight="1">
       <c r="B4" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="36"/>
@@ -2695,139 +2687,139 @@
         <v>8</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N4" s="42"/>
       <c r="O4" s="36"/>
       <c r="P4" s="32"/>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" ht="15.75" customHeight="1">
       <c r="B5" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="O5" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="15.75" customHeight="1">
+      <c r="B6" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>72</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16">
-      <c r="B6" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>75</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
       <c r="J6" s="24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L6" s="24" t="s">
         <v>8</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" ht="15.75" customHeight="1">
       <c r="B7" s="26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G7" s="27">
         <v>10</v>
       </c>
       <c r="H7" s="26"/>
       <c r="J7" s="24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L7" s="24" t="s">
         <v>8</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O7" s="28">
         <v>50</v>
       </c>
       <c r="P7" s="24"/>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" ht="15.75" customHeight="1">
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -2836,21 +2828,21 @@
       <c r="G8" s="30"/>
       <c r="H8" s="29"/>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" ht="15.75" customHeight="1">
       <c r="B9" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>22</v>
@@ -2859,19 +2851,19 @@
         <v>45738</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M9" s="17" t="s">
         <v>21</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O9" s="17" t="s">
         <v>22</v>
@@ -2880,7 +2872,7 @@
         <v>45738</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" ht="15.75" customHeight="1">
       <c r="B10" s="24" t="s">
         <v>9</v>
       </c>
@@ -2888,10 +2880,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F10" s="42"/>
       <c r="G10" s="36"/>
@@ -2900,101 +2892,101 @@
         <v>7</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N10" s="42"/>
       <c r="O10" s="36"/>
       <c r="P10" s="32"/>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" ht="15.75" customHeight="1">
       <c r="B11" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" customHeight="1">
       <c r="B12" s="24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
       <c r="J12" s="24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L12" s="24" t="s">
         <v>7</v>
       </c>
       <c r="M12" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" ht="15.75" customHeight="1">
       <c r="B13" s="24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>9</v>
@@ -3003,34 +2995,34 @@
         <v>9</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G13" s="28"/>
       <c r="H13" s="24"/>
       <c r="J13" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L13" s="24" t="s">
         <v>7</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N13" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O13" s="28">
         <v>50</v>
       </c>
       <c r="P13" s="24"/>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" ht="15.75" customHeight="1">
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -3046,21 +3038,21 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" ht="15.75" customHeight="1">
       <c r="B15" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>22</v>
@@ -3069,19 +3061,19 @@
         <v>45738</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M15" s="17" t="s">
         <v>21</v>
       </c>
       <c r="N15" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O15" s="17" t="s">
         <v>22</v>
@@ -3090,7 +3082,7 @@
         <v>45738</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" ht="15.75" customHeight="1">
       <c r="B16" s="24" t="s">
         <v>11</v>
       </c>
@@ -3098,10 +3090,10 @@
         <v>11</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="36"/>
@@ -3113,110 +3105,110 @@
         <v>5</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N16" s="42"/>
       <c r="O16" s="36"/>
       <c r="P16" s="32"/>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" ht="15.75" customHeight="1">
       <c r="B17" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P17" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="15.75" customHeight="1">
       <c r="B18" s="24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="J18" s="24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L18" s="24" t="s">
         <v>5</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N18" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="24"/>
     </row>
-    <row r="19" spans="2:16">
+    <row r="19" spans="2:16" ht="15.75" customHeight="1">
       <c r="B19" s="24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G19" s="28">
         <v>25</v>
@@ -3225,59 +3217,59 @@
         <v>0</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L19" s="24" t="s">
         <v>5</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O19" s="28">
         <v>50</v>
       </c>
       <c r="P19" s="24"/>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:16" ht="15.75" customHeight="1">
       <c r="J20" s="24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L20" s="24" t="s">
         <v>5</v>
       </c>
       <c r="M20" s="24"/>
       <c r="N20" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O20" s="28">
         <v>10</v>
       </c>
       <c r="P20" s="24"/>
     </row>
-    <row r="21" spans="2:16">
+    <row r="21" spans="2:16" ht="15.75" customHeight="1">
       <c r="B21" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>22</v>
@@ -3286,38 +3278,38 @@
         <v>45738</v>
       </c>
     </row>
-    <row r="22" spans="2:16">
+    <row r="22" spans="2:16" ht="15.75" customHeight="1">
       <c r="B22" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F22" s="42" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G22" s="36"/>
       <c r="H22" s="32"/>
       <c r="J22" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M22" s="17" t="s">
         <v>21</v>
       </c>
       <c r="N22" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O22" s="17" t="s">
         <v>22</v>
@@ -3326,27 +3318,27 @@
         <v>45738</v>
       </c>
     </row>
-    <row r="23" spans="2:16">
+    <row r="23" spans="2:16" ht="15.75" customHeight="1">
       <c r="B23" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J23" s="24" t="s">
         <v>10</v>
@@ -3355,99 +3347,99 @@
         <v>10</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N23" s="42"/>
       <c r="O23" s="36"/>
       <c r="P23" s="32"/>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:16" ht="15.75" customHeight="1">
       <c r="B24" s="24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
       <c r="J24" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L24" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N24" s="17" t="s">
         <v>8</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="15.75" customHeight="1">
       <c r="B25" s="24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G25" s="28">
         <v>255</v>
       </c>
       <c r="H25" s="24"/>
       <c r="J25" s="24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L25" s="24" t="s">
         <v>10</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N25" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
     </row>
-    <row r="26" spans="2:16">
+    <row r="26" spans="2:16" ht="15.75" customHeight="1">
       <c r="B26" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>6</v>
@@ -3459,29 +3451,29 @@
       <c r="G26" s="28"/>
       <c r="H26" s="24"/>
       <c r="J26" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L26" s="24" t="s">
         <v>10</v>
       </c>
       <c r="M26" s="24"/>
       <c r="N26" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O26" s="28">
         <v>10</v>
       </c>
       <c r="P26" s="24"/>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:16" ht="15.75" customHeight="1">
       <c r="B27" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>6</v>
@@ -3493,17 +3485,17 @@
       <c r="G27" s="28"/>
       <c r="H27" s="24"/>
       <c r="J27" s="24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L27" s="24" t="s">
         <v>10</v>
       </c>
       <c r="M27" s="24"/>
       <c r="N27" s="24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O27" s="28">
         <v>3</v>
@@ -3512,118 +3504,118 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:16">
+    <row r="28" spans="2:16" ht="15.75" customHeight="1">
       <c r="B28" s="24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D28" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G28" s="28"/>
       <c r="H28" s="24"/>
       <c r="J28" s="24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L28" s="24" t="s">
         <v>10</v>
       </c>
       <c r="M28" s="24"/>
       <c r="N28" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O28" s="28">
         <v>30</v>
       </c>
       <c r="P28" s="24"/>
     </row>
-    <row r="29" spans="2:16">
+    <row r="29" spans="2:16" ht="15.75" customHeight="1">
       <c r="B29" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D29" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G29" s="28">
         <v>50</v>
       </c>
       <c r="H29" s="24"/>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:16" ht="15.75" customHeight="1">
       <c r="B30" s="24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G30" s="28"/>
       <c r="H30" s="24"/>
     </row>
-    <row r="31" spans="2:16">
+    <row r="31" spans="2:16" ht="15.75" customHeight="1">
       <c r="B31" s="24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G31" s="28">
         <v>50</v>
       </c>
       <c r="H31" s="24"/>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" ht="15.75" customHeight="1">
       <c r="B33" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>21</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>22</v>
@@ -3632,94 +3624,94 @@
         <v>45738</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" ht="13">
       <c r="B34" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F34" s="42" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G34" s="36"/>
       <c r="H34" s="32"/>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" ht="13">
       <c r="B35" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="13">
       <c r="B36" s="24" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" ht="13">
       <c r="B37" s="24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G37" s="28">
         <v>255</v>
       </c>
       <c r="H37" s="24"/>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" ht="13">
       <c r="B38" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>4</v>
@@ -3731,12 +3723,12 @@
       <c r="G38" s="28"/>
       <c r="H38" s="24"/>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" ht="13">
       <c r="B39" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>4</v>
@@ -3748,120 +3740,120 @@
       <c r="G39" s="28"/>
       <c r="H39" s="24"/>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" ht="13">
       <c r="B40" s="24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="24"/>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" ht="13">
       <c r="B41" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G41" s="28">
         <v>3</v>
       </c>
       <c r="H41" s="24"/>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="2:8" ht="13">
       <c r="B42" s="24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="24"/>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" ht="13">
       <c r="B43" s="24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G43" s="28">
         <v>50</v>
       </c>
       <c r="H43" s="24"/>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:8" ht="13">
       <c r="B44" s="24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D44" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G44" s="28"/>
       <c r="H44" s="24"/>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" ht="13">
       <c r="B45" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D45" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G45" s="28">
         <v>50</v>

</xml_diff>